<commit_message>
AD updates for item groups
</commit_message>
<xml_diff>
--- a/Data Extraction And Loading/Import Files/Retail Item/Retail Item Import Template.xlsx
+++ b/Data Extraction And Loading/Import Files/Retail Item/Retail Item Import Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck\Documents\ROC\Data Extraction and Loading\Import Files\Retail Item\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\15_Work_ROC\50_Client_01_Speedway\90_Testing_Code\Data Extraction And Loading\Import Files\Retail Item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A96324-7B4C-4208-B9B0-88720032FB1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE7D69F-C35C-466D-85CA-442AF4523457}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21825" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="85">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -257,6 +257,24 @@
   </si>
   <si>
     <t>Puged in BC</t>
+  </si>
+  <si>
+    <t>Item Groups</t>
+  </si>
+  <si>
+    <t>Item Group #1</t>
+  </si>
+  <si>
+    <t>Item Group #2</t>
+  </si>
+  <si>
+    <t>Item Group #3</t>
+  </si>
+  <si>
+    <t>Item Group #4</t>
+  </si>
+  <si>
+    <t>Item Group #5</t>
   </si>
 </sst>
 </file>
@@ -399,7 +417,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +648,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -952,7 +976,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1020,6 +1044,9 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1077,8 +1104,26 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1127,6 +1172,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1435,95 +1485,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CY4"/>
+  <dimension ref="A1:DD4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="9.265625" customWidth="1"/>
+    <col min="3" max="3" width="27.86328125" customWidth="1"/>
+    <col min="4" max="4" width="17.1328125" customWidth="1"/>
+    <col min="5" max="5" width="7.265625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.265625" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.3984375" customWidth="1"/>
+    <col min="10" max="10" width="14.3984375" customWidth="1"/>
+    <col min="11" max="11" width="17.86328125" customWidth="1"/>
+    <col min="13" max="13" width="14.1328125" customWidth="1"/>
+    <col min="15" max="15" width="10.1328125" customWidth="1"/>
+    <col min="16" max="16" width="16.265625" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
     <col min="31" max="31" width="11" customWidth="1"/>
     <col min="32" max="32" width="9" customWidth="1"/>
-    <col min="35" max="35" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="10.73046875" customWidth="1"/>
     <col min="39" max="39" width="12" customWidth="1"/>
-    <col min="41" max="41" width="8.85546875" style="15"/>
-    <col min="43" max="43" width="19.28515625" style="13" customWidth="1"/>
-    <col min="44" max="44" width="15.7109375" customWidth="1"/>
-    <col min="45" max="45" width="15.7109375" style="6" customWidth="1"/>
-    <col min="46" max="103" width="15.7109375" customWidth="1"/>
+    <col min="41" max="41" width="8.86328125" style="15"/>
+    <col min="43" max="43" width="19.265625" style="13" customWidth="1"/>
+    <col min="44" max="44" width="15.73046875" customWidth="1"/>
+    <col min="45" max="45" width="15.73046875" style="6" customWidth="1"/>
+    <col min="46" max="103" width="15.73046875" customWidth="1"/>
+    <col min="104" max="108" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:108" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="18"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="38" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="41" t="s">
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
-      <c r="AC1" s="42"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="35" t="s">
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
-      <c r="AO1" s="36"/>
-      <c r="AP1" s="36"/>
-      <c r="AQ1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="37"/>
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="38"/>
       <c r="AR1" s="22" t="s">
         <v>69</v>
       </c>
@@ -1586,8 +1637,15 @@
       <c r="CW1" s="23"/>
       <c r="CX1" s="23"/>
       <c r="CY1" s="24"/>
+      <c r="CZ1" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="DA1" s="49"/>
+      <c r="DB1" s="49"/>
+      <c r="DC1" s="49"/>
+      <c r="DD1" s="50"/>
     </row>
-    <row r="2" spans="1:103" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:108" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>18</v>
       </c>
@@ -1630,159 +1688,164 @@
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
       <c r="T2" s="12"/>
-      <c r="U2" s="41" t="s">
+      <c r="U2" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="41" t="s">
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="32" t="s">
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="30" t="s">
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="31"/>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="31"/>
-      <c r="AP2" s="31"/>
-      <c r="AQ2" s="31"/>
-      <c r="AR2" s="25" t="s">
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="AS2" s="25"/>
-      <c r="AT2" s="25" t="s">
+      <c r="AS2" s="26"/>
+      <c r="AT2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AU2" s="25"/>
-      <c r="AV2" s="25" t="s">
+      <c r="AU2" s="26"/>
+      <c r="AV2" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="AW2" s="25"/>
-      <c r="AX2" s="26" t="s">
+      <c r="AW2" s="26"/>
+      <c r="AX2" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="AY2" s="26"/>
-      <c r="AZ2" s="25" t="s">
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="BA2" s="25"/>
-      <c r="BB2" s="25" t="s">
+      <c r="BA2" s="26"/>
+      <c r="BB2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="BC2" s="25"/>
-      <c r="BD2" s="25" t="s">
+      <c r="BC2" s="26"/>
+      <c r="BD2" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="BE2" s="25"/>
-      <c r="BF2" s="25" t="s">
+      <c r="BE2" s="26"/>
+      <c r="BF2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="BG2" s="25"/>
-      <c r="BH2" s="26" t="s">
+      <c r="BG2" s="26"/>
+      <c r="BH2" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="BI2" s="26"/>
-      <c r="BJ2" s="25" t="s">
+      <c r="BI2" s="27"/>
+      <c r="BJ2" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="BK2" s="25"/>
-      <c r="BL2" s="25" t="s">
+      <c r="BK2" s="26"/>
+      <c r="BL2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="BM2" s="25"/>
-      <c r="BN2" s="25" t="s">
+      <c r="BM2" s="26"/>
+      <c r="BN2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="BO2" s="25"/>
-      <c r="BP2" s="25" t="s">
+      <c r="BO2" s="26"/>
+      <c r="BP2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="BQ2" s="25"/>
-      <c r="BR2" s="26" t="s">
+      <c r="BQ2" s="26"/>
+      <c r="BR2" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="BS2" s="26"/>
-      <c r="BT2" s="25" t="s">
+      <c r="BS2" s="27"/>
+      <c r="BT2" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="BU2" s="25"/>
-      <c r="BV2" s="25" t="s">
+      <c r="BU2" s="26"/>
+      <c r="BV2" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="BW2" s="25"/>
-      <c r="BX2" s="25" t="s">
+      <c r="BW2" s="26"/>
+      <c r="BX2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="BY2" s="25"/>
-      <c r="BZ2" s="25" t="s">
+      <c r="BY2" s="26"/>
+      <c r="BZ2" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="CA2" s="25"/>
-      <c r="CB2" s="26" t="s">
+      <c r="CA2" s="26"/>
+      <c r="CB2" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="CC2" s="26"/>
-      <c r="CD2" s="25" t="s">
+      <c r="CC2" s="27"/>
+      <c r="CD2" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="CE2" s="25"/>
-      <c r="CF2" s="25" t="s">
+      <c r="CE2" s="26"/>
+      <c r="CF2" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="CG2" s="25"/>
-      <c r="CH2" s="25" t="s">
+      <c r="CG2" s="26"/>
+      <c r="CH2" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="CI2" s="25"/>
-      <c r="CJ2" s="25" t="s">
+      <c r="CI2" s="26"/>
+      <c r="CJ2" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="CK2" s="25"/>
-      <c r="CL2" s="26" t="s">
+      <c r="CK2" s="26"/>
+      <c r="CL2" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="CM2" s="26"/>
-      <c r="CN2" s="25" t="s">
+      <c r="CM2" s="27"/>
+      <c r="CN2" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="CO2" s="25"/>
-      <c r="CP2" s="25" t="s">
+      <c r="CO2" s="26"/>
+      <c r="CP2" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="CQ2" s="25"/>
-      <c r="CR2" s="25" t="s">
+      <c r="CQ2" s="26"/>
+      <c r="CR2" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="CS2" s="25"/>
-      <c r="CT2" s="25" t="s">
+      <c r="CS2" s="26"/>
+      <c r="CT2" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="CU2" s="25"/>
-      <c r="CV2" s="26" t="s">
+      <c r="CU2" s="26"/>
+      <c r="CV2" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="CW2" s="26"/>
-      <c r="CX2" s="25" t="s">
+      <c r="CW2" s="27"/>
+      <c r="CX2" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="CY2" s="25"/>
+      <c r="CY2" s="26"/>
+      <c r="CZ2" s="46"/>
+      <c r="DA2" s="47"/>
+      <c r="DB2" s="47"/>
+      <c r="DC2" s="47"/>
+      <c r="DD2" s="48"/>
     </row>
-    <row r="3" spans="1:103" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:108" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="3"/>
@@ -2070,18 +2133,54 @@
       <c r="CY3" s="21" t="s">
         <v>43</v>
       </c>
+      <c r="CZ3" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="DA3" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="DB3" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="DC3" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="DD3" s="51" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:108" x14ac:dyDescent="0.45">
       <c r="AO4"/>
       <c r="AQ4"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
+  <mergeCells count="39">
+    <mergeCell ref="CZ1:DD1"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CX2:CY2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
     <mergeCell ref="C1:K1"/>
     <mergeCell ref="AK2:AQ2"/>
     <mergeCell ref="AE2:AJ2"/>
@@ -2090,31 +2189,11 @@
     <mergeCell ref="U1:AD1"/>
     <mergeCell ref="U2:Y2"/>
     <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CX2:CY2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>